<commit_message>
completed the code for testing
</commit_message>
<xml_diff>
--- a/pages/Bangalore.xlsx
+++ b/pages/Bangalore.xlsx
@@ -8,14 +8,13 @@
   </bookViews>
   <sheets>
     <sheet name="dance" sheetId="1" r:id="rId1"/>
-    <sheet name="yoga" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>DESCRIPTION</t>
   </si>
@@ -44,25 +43,31 @@
     <t>NAME</t>
   </si>
   <si>
-    <t>Bodhi Yoga Academy - AECS Layout</t>
-  </si>
-  <si>
-    <t>Get fit and train others! We offer daily yoga classes as well as RYT200 Teacher Training by our expert faculty. Bodhi Yoga at AECS Layout has become the best rated Yoga Studio in Bangalore within a Short Time. Come for a trial class and see for yourself!</t>
-  </si>
-  <si>
-    <t>1,117 people</t>
-  </si>
-  <si>
-    <t>1,132 people follow this</t>
-  </si>
-  <si>
-    <t>302, 60 Ft Main Road, AECS Layout Bangalore, India 560037</t>
-  </si>
-  <si>
-    <t>https://www.facebook.com/BodhiAECSLayout/</t>
-  </si>
-  <si>
-    <t>Yoga</t>
+    <t>Rhythmic Feet Dance Academy Private Limited</t>
+  </si>
+  <si>
+    <t>Rhythmic Feet Dance Academy Private Limited is a dance and fitness studio, owned By Julie Masih based out of Koramangala, Bangalore.</t>
+  </si>
+  <si>
+    <t>6,930 people</t>
+  </si>
+  <si>
+    <t>7,104 people follow this</t>
+  </si>
+  <si>
+    <t>https://www.rhythmicfeetpvtltd.com/</t>
+  </si>
+  <si>
+    <t>098804 34385</t>
+  </si>
+  <si>
+    <t>Bangalore, India 560095</t>
+  </si>
+  <si>
+    <t>https://www.facebook.com/rhythmicfeet/</t>
+  </si>
+  <si>
+    <t>Western</t>
   </si>
 </sst>
 </file>
@@ -433,7 +438,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -468,48 +473,6 @@
         <v>7</v>
       </c>
     </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1" spans="1:9">
-      <c r="A1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="2" spans="1:9">
       <c r="A2" s="1" t="s">
         <v>9</v>
@@ -523,19 +486,26 @@
       <c r="D2" t="s">
         <v>12</v>
       </c>
+      <c r="E2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="I2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="H2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>